<commit_message>
Transformation function for DUKES 1.3
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_1.xlsx
+++ b/data/templates/dukes_ch_1.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43CE59B1-4BF1-47C2-9B4A-6F6DD3ECF294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE4E726-3D0C-4EEA-A5EC-B7669C055ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.3.A" sheetId="1" r:id="rId1"/>
-    <sheet name="1-1-B" sheetId="3" r:id="rId2"/>
+    <sheet name="1.3.B" sheetId="3" r:id="rId2"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -977,7 +977,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Transformation for table 1.1.1
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_1.xlsx
+++ b/data/templates/dukes_ch_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE4E726-3D0C-4EEA-A5EC-B7669C055ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8280F870-8B51-41CF-9EE8-2B2CD2370C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.3.A" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="67">
   <si>
     <t>Electricity generation - Gas</t>
   </si>
@@ -143,47 +143,98 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Worksheet description</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Cover sheet</t>
-  </si>
-  <si>
-    <t>Cover Sheet</t>
-  </si>
-  <si>
-    <t>Contents</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Sales of electricity and gas by sector, United Kingdom, Total selling value £ million</t>
-  </si>
-  <si>
-    <t>1.3.A</t>
-  </si>
-  <si>
-    <t>Sales of electricity and gas by sector, United Kingdom, Average net selling value per kWh sold (pence)</t>
-  </si>
-  <si>
-    <t>1.3.B</t>
-  </si>
-  <si>
     <t>million GBP</t>
   </si>
   <si>
     <t>pence per kWh</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Natural gas</t>
+  </si>
+  <si>
+    <t>Total Imports</t>
+  </si>
+  <si>
+    <t>Petroleum, Marine Bunkers</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>Exports</t>
+  </si>
+  <si>
+    <t>Marine bunkers</t>
+  </si>
+  <si>
+    <t>Stock Change [note note 8]</t>
+  </si>
+  <si>
+    <t>Statistical Difference [note note 10]</t>
+  </si>
+  <si>
+    <t>Gross inland consumption</t>
+  </si>
+  <si>
+    <t>Non energy use</t>
+  </si>
+  <si>
+    <t>Inland consumption for energy use</t>
+  </si>
+  <si>
+    <t>Petroleum</t>
+  </si>
+  <si>
+    <t>Primary electricity</t>
+  </si>
+  <si>
+    <t>Total Production</t>
+  </si>
+  <si>
+    <t>Total Exports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coal, Stock Change </t>
+  </si>
+  <si>
+    <t>Petroleum, Stock Change</t>
+  </si>
+  <si>
+    <t>Natural gas, Stock Change</t>
+  </si>
+  <si>
+    <t>Total Statistical Difference</t>
+  </si>
+  <si>
+    <t>Gross Inland Consumption</t>
+  </si>
+  <si>
+    <t>Non Energy Use</t>
+  </si>
+  <si>
+    <t>Total Inland Consumption for Energy Use</t>
+  </si>
+  <si>
+    <t>ktoe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,16 +242,382 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -208,15 +625,226 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="55">
+    <cellStyle name="20% - Colore 1 2" xfId="19" xr:uid="{AF6480ED-A694-4FFF-95F1-9AF482CC0E86}"/>
+    <cellStyle name="20% - Colore 2 2" xfId="23" xr:uid="{EB88AE67-47E5-4A82-BE66-27C0D6D2FC2E}"/>
+    <cellStyle name="20% - Colore 3 2" xfId="27" xr:uid="{807784AA-763E-4784-96AF-4E54AF45863C}"/>
+    <cellStyle name="20% - Colore 4 2" xfId="31" xr:uid="{4C496E3B-BD22-4C04-B475-AF97E95EE3CD}"/>
+    <cellStyle name="20% - Colore 5 2" xfId="35" xr:uid="{A974C6C5-E4EE-405F-B6E1-C38E91709A11}"/>
+    <cellStyle name="20% - Colore 6 2" xfId="39" xr:uid="{1B77E8D2-7BFF-4CE8-B4AC-2706A5D3E6EC}"/>
+    <cellStyle name="40% - Colore 1 2" xfId="20" xr:uid="{7F210A86-B23B-40F1-A6FA-CB68EC38A860}"/>
+    <cellStyle name="40% - Colore 2 2" xfId="24" xr:uid="{97E4AE9B-DB13-474F-9524-99BDBC897B5B}"/>
+    <cellStyle name="40% - Colore 3 2" xfId="28" xr:uid="{EEF4AEF3-B1F9-4BC7-AA37-C055268A64BD}"/>
+    <cellStyle name="40% - Colore 4 2" xfId="32" xr:uid="{F1B38282-8139-44B7-8F3C-4186D92BB043}"/>
+    <cellStyle name="40% - Colore 5 2" xfId="36" xr:uid="{BCF9BAB9-0ED8-403B-96C2-0E9DEC11575C}"/>
+    <cellStyle name="40% - Colore 6 2" xfId="40" xr:uid="{CD8B45D9-FFE7-49A5-A165-372E1DBC8372}"/>
+    <cellStyle name="60% - Colore 1 2" xfId="21" xr:uid="{8AA2DE33-0029-4128-8B10-68DB36206C47}"/>
+    <cellStyle name="60% - Colore 2 2" xfId="25" xr:uid="{BCF4F08B-A0AA-4A72-A8F3-7CC0597C240C}"/>
+    <cellStyle name="60% - Colore 3 2" xfId="29" xr:uid="{6D67A112-4C4A-449E-A939-529B3745B6B9}"/>
+    <cellStyle name="60% - Colore 4 2" xfId="33" xr:uid="{DD6AEC98-ED97-4DE3-AEF7-D5892518EA19}"/>
+    <cellStyle name="60% - Colore 5 2" xfId="37" xr:uid="{9108657F-D7C1-4C3F-BEE5-317E106FF268}"/>
+    <cellStyle name="60% - Colore 6 2" xfId="41" xr:uid="{1A99EC43-5728-465D-B97D-98026697850B}"/>
+    <cellStyle name="Calcolo 2" xfId="12" xr:uid="{04D4A835-83E1-4AD9-9E89-83112820C8C2}"/>
+    <cellStyle name="Cella collegata 2" xfId="13" xr:uid="{92188C2D-ACA1-412D-981A-97785C31F887}"/>
+    <cellStyle name="Cella da controllare 2" xfId="14" xr:uid="{6FEED1AB-76D3-48B4-B9C8-7CC11C3F6DBA}"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="42" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="43" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Colore 1 2" xfId="18" xr:uid="{3CB4ED0D-76AA-43A3-83CD-3FADD6D63009}"/>
+    <cellStyle name="Colore 2 2" xfId="22" xr:uid="{AB5EA218-BFBA-4F02-8AB1-824A31155C54}"/>
+    <cellStyle name="Colore 3 2" xfId="26" xr:uid="{FE2C67B9-E0E2-43B3-A1A5-131FA15B278F}"/>
+    <cellStyle name="Colore 4 2" xfId="30" xr:uid="{E5D675BA-2DF8-43B2-95F2-E33B8C7B959A}"/>
+    <cellStyle name="Colore 5 2" xfId="34" xr:uid="{F6C20180-31E1-4B63-B88E-EE6004D71AE5}"/>
+    <cellStyle name="Colore 6 2" xfId="38" xr:uid="{8B5E8239-18B4-4DA4-92D5-11F989FF6729}"/>
+    <cellStyle name="Heading 1 2" xfId="44" xr:uid="{3F4110AC-9E7B-4449-A52E-254543C04E7B}"/>
+    <cellStyle name="Heading 2 2" xfId="46" xr:uid="{F2FF1017-97E3-495E-AF32-0438546316F1}"/>
+    <cellStyle name="Heading 3 2" xfId="48" xr:uid="{C1A83283-B929-4810-8AA0-FDF032C9C42B}"/>
+    <cellStyle name="Hyperlink 2" xfId="47" xr:uid="{AF792365-A4BB-44FA-8C38-AB41663EA6E6}"/>
+    <cellStyle name="Hyperlink 3" xfId="50" xr:uid="{664321C9-C614-4630-B351-271614424B6E}"/>
+    <cellStyle name="Input 2" xfId="10" xr:uid="{EEAC3A53-F414-4198-A5C8-D3831B9F3DB2}"/>
+    <cellStyle name="Neutrale 2" xfId="9" xr:uid="{74628F60-C1EB-49B6-87EA-52EDD00C6FA0}"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{B3AE7470-ADDF-45D4-9CF5-1BDAD10E5F12}"/>
+    <cellStyle name="Normal 2 2" xfId="49" xr:uid="{312D4C7A-4071-4588-9816-FD37789C0722}"/>
+    <cellStyle name="Normal 2 3" xfId="52" xr:uid="{2D4CCCDF-B7AC-4C13-B6A6-349943D7226D}"/>
+    <cellStyle name="Normal 3" xfId="53" xr:uid="{4D3212D7-9D95-43A1-B7BE-4F430AA474CB}"/>
+    <cellStyle name="Normal 4" xfId="45" xr:uid="{C36E3D9A-05ED-4C97-B0BA-F48297BAEE28}"/>
+    <cellStyle name="Normal 8" xfId="54" xr:uid="{832E45CD-2FBB-4ECF-8326-6E9CE4248DFE}"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale 2" xfId="1" xr:uid="{CA944CA4-9248-4D6A-96A0-CA7E20293B6D}"/>
+    <cellStyle name="Output 2" xfId="11" xr:uid="{717A4618-5F73-4708-97D7-5B8256DDEDAA}"/>
+    <cellStyle name="Testo avviso 2" xfId="15" xr:uid="{BC41BAFB-F80C-43B6-BD54-003670C4631B}"/>
+    <cellStyle name="Testo descrittivo 2" xfId="16" xr:uid="{6B9FE4ED-7FB5-4DF5-8229-46648CDDD868}"/>
+    <cellStyle name="Titolo 1 2" xfId="3" xr:uid="{73DAB657-F0F8-4637-B78C-87D09FD46893}"/>
+    <cellStyle name="Titolo 2 2" xfId="4" xr:uid="{7D4A08AF-E382-48E6-8607-A5E831BC48C1}"/>
+    <cellStyle name="Titolo 3 2" xfId="5" xr:uid="{411FCC39-F1DC-4EB7-8361-DB3A3EDC5F73}"/>
+    <cellStyle name="Titolo 4 2" xfId="6" xr:uid="{970F5741-486C-4EC1-B7F1-43AF8825D56E}"/>
+    <cellStyle name="Titolo 5" xfId="2" xr:uid="{6A35A386-FD55-4C02-95A6-61A79AD67B33}"/>
+    <cellStyle name="Totale 2" xfId="17" xr:uid="{CAC87389-C147-4A18-B323-E6A560026CE0}"/>
+    <cellStyle name="Valore non valido 2" xfId="8" xr:uid="{E228C974-A134-4A8D-931D-CE78F28A34D9}"/>
+    <cellStyle name="Valore valido 2" xfId="7" xr:uid="{FD376C03-DCE2-4500-B3A5-870AD4F41220}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -644,7 +1272,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -664,7 +1292,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -684,7 +1312,7 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -704,7 +1332,7 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -724,7 +1352,7 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -744,7 +1372,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -764,7 +1392,7 @@
         <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -784,7 +1412,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -804,7 +1432,7 @@
         <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -824,7 +1452,7 @@
         <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -844,7 +1472,7 @@
         <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -864,7 +1492,7 @@
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -884,7 +1512,7 @@
         <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -904,7 +1532,7 @@
         <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -924,7 +1552,7 @@
         <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -944,7 +1572,7 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -964,7 +1592,7 @@
         <v>27</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -976,7 +1604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4341AC-9278-4308-B637-81E7010F9C46}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1019,7 +1647,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1039,7 +1667,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1059,7 +1687,7 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1079,7 +1707,7 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1099,7 +1727,7 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1119,7 +1747,7 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1139,7 +1767,7 @@
         <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1159,7 +1787,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1179,7 +1807,7 @@
         <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1199,7 +1827,7 @@
         <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1219,7 +1847,7 @@
         <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1239,7 +1867,7 @@
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1259,7 +1887,7 @@
         <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1279,7 +1907,7 @@
         <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1299,7 +1927,7 @@
         <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1319,7 +1947,7 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1339,7 +1967,7 @@
         <v>27</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1349,75 +1977,491 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1026899-EDF0-43C7-8585-EB7C14354B18}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
       <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
-        <v>46</v>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continuing chapter 1 transformations
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_1.xlsx
+++ b/data/templates/dukes_ch_1.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC243DA8-E476-4084-BF49-48EB3D3B2B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16784A7-3AE9-451B-A3F4-6DA30CFA694A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.3.A" sheetId="1" r:id="rId1"/>
-    <sheet name="1.3.B" sheetId="3" r:id="rId2"/>
-    <sheet name="1.1.A" sheetId="4" r:id="rId3"/>
-    <sheet name="1.1.B" sheetId="5" r:id="rId4"/>
-    <sheet name="1.1.C" sheetId="6" r:id="rId5"/>
-    <sheet name="1.1.2" sheetId="2" r:id="rId6"/>
+    <sheet name="1.1" sheetId="10" r:id="rId2"/>
+    <sheet name="1.3.B" sheetId="3" r:id="rId3"/>
+    <sheet name="1.1.A" sheetId="4" r:id="rId4"/>
+    <sheet name="1.1.B" sheetId="5" r:id="rId5"/>
+    <sheet name="1.1.C" sheetId="6" r:id="rId6"/>
+    <sheet name="1.1.2" sheetId="2" r:id="rId7"/>
+    <sheet name="1.1.3" sheetId="7" r:id="rId8"/>
+    <sheet name="1.1.4" sheetId="8" r:id="rId9"/>
+    <sheet name="1.1.5" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="183">
   <si>
     <t>Electricity generation - Gas</t>
   </si>
@@ -258,6 +262,327 @@
   </si>
   <si>
     <t>Fossil fuel dependency</t>
+  </si>
+  <si>
+    <t>Gross inland consumption of primary fuels plus marine bunkers, million tonnes of oil equivalent [note 1]</t>
+  </si>
+  <si>
+    <t>Net imports/net exports of fuels, million tonnes of oil equivalent [note 2]</t>
+  </si>
+  <si>
+    <t>Import dependency, percentage [note 3]</t>
+  </si>
+  <si>
+    <t>Export dependency, percentage [note 4]</t>
+  </si>
+  <si>
+    <t>Gross inland consumption - primary fuels and marine bunkers</t>
+  </si>
+  <si>
+    <t>Net imports/net exports of fuels</t>
+  </si>
+  <si>
+    <t>Import dependency</t>
+  </si>
+  <si>
+    <t>Export dependency</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Total inland consumption of primary energy (temperature corrected), million tonnes of oil equivalent</t>
+  </si>
+  <si>
+    <t>Gross Domestic Product (GDP) chained volume measure (2019 prices), £billion</t>
+  </si>
+  <si>
+    <t>Energy ratio, tonnes of oil equivalent per £1 million GDP, percentage [note 1]</t>
+  </si>
+  <si>
+    <t>Index 1970=100</t>
+  </si>
+  <si>
+    <t>Total infland consumption of primary fuels (temperature adjusted)</t>
+  </si>
+  <si>
+    <t>GDP chained volume measure</t>
+  </si>
+  <si>
+    <t>Energy ratio</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>toe per million GBP</t>
+  </si>
+  <si>
+    <t>percent (1970 = 100)</t>
+  </si>
+  <si>
+    <t>Industry: Coal and solid fuels [note 2]</t>
+  </si>
+  <si>
+    <t>Industry: Natural gas [note 3]</t>
+  </si>
+  <si>
+    <t>Industry: Electricity</t>
+  </si>
+  <si>
+    <t>Industry: Petroleum products [note 4]</t>
+  </si>
+  <si>
+    <t>Industry: Heat and other fuels [note 5]</t>
+  </si>
+  <si>
+    <t>Total Industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic: Coal and solid fuels [note 2] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic: Natural gas [note 3] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic: Electricity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic: Petroleum products [note 4] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic: Heat and other fuels [note 5] </t>
+  </si>
+  <si>
+    <t>Total Domestic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other Final Users: Coal and solid fuels [note 2]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other Final Users: Natural gas [note 3]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other Final Users: Electricity  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other Final Users: Petroleum products [note 4]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other Final Users: of which road transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other Final Users: Heat and other fuels [note 5]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Other Final Users [note 6] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Final Users: Coal and solid fuels [note 2]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Final Users: Natural gas [note 3]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Final Users: Electricity   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Final Users: Petroleum products [note 4]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Final Users: Heat and other fuels [note 5]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total All Final Users </t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>subsector</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Coal and solid fuels</t>
+  </si>
+  <si>
+    <t>Petroleum products</t>
+  </si>
+  <si>
+    <t>Heat and other fuels</t>
+  </si>
+  <si>
+    <t>All fuels</t>
+  </si>
+  <si>
+    <t>Other final users</t>
+  </si>
+  <si>
+    <t>Road transport</t>
+  </si>
+  <si>
+    <t>All sectors</t>
+  </si>
+  <si>
+    <t>All subsectors</t>
+  </si>
+  <si>
+    <t>Stock change [note 4]</t>
+  </si>
+  <si>
+    <t>Total supply</t>
+  </si>
+  <si>
+    <t>Statistical difference [note 5]</t>
+  </si>
+  <si>
+    <t>Total demand</t>
+  </si>
+  <si>
+    <t>Transfers</t>
+  </si>
+  <si>
+    <t>Transformation</t>
+  </si>
+  <si>
+    <t>Major power producers</t>
+  </si>
+  <si>
+    <t>Autogenerators</t>
+  </si>
+  <si>
+    <t>Heat generation</t>
+  </si>
+  <si>
+    <t>Petroleum refineries</t>
+  </si>
+  <si>
+    <t>Coke manufacture</t>
+  </si>
+  <si>
+    <t>Blast furnaces</t>
+  </si>
+  <si>
+    <t>Patent fuel manufacture</t>
+  </si>
+  <si>
+    <t>Other [note 6]</t>
+  </si>
+  <si>
+    <t>Energy industry use</t>
+  </si>
+  <si>
+    <t>Oil and gas extraction</t>
+  </si>
+  <si>
+    <t>Coal extraction</t>
+  </si>
+  <si>
+    <t>Storage [note 7]</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>Final consumption</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>Iron and steel</t>
+  </si>
+  <si>
+    <t>Non-ferrous metals</t>
+  </si>
+  <si>
+    <t>Mineral products</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Mechanical engineering etc</t>
+  </si>
+  <si>
+    <t>Electrical engineering etc</t>
+  </si>
+  <si>
+    <t>Vehicles</t>
+  </si>
+  <si>
+    <t>Food, beverages etc</t>
+  </si>
+  <si>
+    <t>Textiles, leather etc</t>
+  </si>
+  <si>
+    <t>Paper, printing etc</t>
+  </si>
+  <si>
+    <t>Other industries</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Rail</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>National navigation</t>
+  </si>
+  <si>
+    <t>Pipelines</t>
+  </si>
+  <si>
+    <t>Public administration</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>subgroup</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Statistical difference</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>flow</t>
+  </si>
+  <si>
+    <t>Stock change</t>
+  </si>
+  <si>
+    <t>Storage</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +1955,1624 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D425282C-868D-490E-98D9-DD5403F8543C}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D05EE7-8D8D-45F8-9599-5A89EAB3B8C2}">
+  <dimension ref="A1:G59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" t="s">
+        <v>179</v>
+      </c>
+      <c r="D17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" t="s">
+        <v>147</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" t="s">
+        <v>147</v>
+      </c>
+      <c r="F24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" t="s">
+        <v>179</v>
+      </c>
+      <c r="D25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" t="s">
+        <v>147</v>
+      </c>
+      <c r="F26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" t="s">
+        <v>147</v>
+      </c>
+      <c r="F27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>179</v>
+      </c>
+      <c r="D30" t="s">
+        <v>147</v>
+      </c>
+      <c r="F30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s">
+        <v>179</v>
+      </c>
+      <c r="D33" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>153</v>
+      </c>
+      <c r="C34" t="s">
+        <v>179</v>
+      </c>
+      <c r="D34" t="s">
+        <v>152</v>
+      </c>
+      <c r="E34" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" t="s">
+        <v>179</v>
+      </c>
+      <c r="D35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" t="s">
+        <v>179</v>
+      </c>
+      <c r="D37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" t="s">
+        <v>179</v>
+      </c>
+      <c r="D38" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>158</v>
+      </c>
+      <c r="C39" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" t="s">
+        <v>124</v>
+      </c>
+      <c r="F39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>159</v>
+      </c>
+      <c r="C40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" t="s">
+        <v>124</v>
+      </c>
+      <c r="F40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" t="s">
+        <v>179</v>
+      </c>
+      <c r="D41" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" t="s">
+        <v>124</v>
+      </c>
+      <c r="F41" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" t="s">
+        <v>179</v>
+      </c>
+      <c r="D42" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" t="s">
+        <v>179</v>
+      </c>
+      <c r="D43" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" t="s">
+        <v>124</v>
+      </c>
+      <c r="F44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" t="s">
+        <v>179</v>
+      </c>
+      <c r="D45" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" t="s">
+        <v>179</v>
+      </c>
+      <c r="D46" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>179</v>
+      </c>
+      <c r="D47" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" t="s">
+        <v>179</v>
+      </c>
+      <c r="D48" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" t="s">
+        <v>179</v>
+      </c>
+      <c r="D49" t="s">
+        <v>152</v>
+      </c>
+      <c r="E49" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" t="s">
+        <v>179</v>
+      </c>
+      <c r="D50" t="s">
+        <v>152</v>
+      </c>
+      <c r="E50" t="s">
+        <v>31</v>
+      </c>
+      <c r="F50" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>169</v>
+      </c>
+      <c r="C51" t="s">
+        <v>179</v>
+      </c>
+      <c r="D51" t="s">
+        <v>152</v>
+      </c>
+      <c r="E51" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>170</v>
+      </c>
+      <c r="C52" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" t="s">
+        <v>152</v>
+      </c>
+      <c r="E52" t="s">
+        <v>31</v>
+      </c>
+      <c r="F52" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" t="s">
+        <v>152</v>
+      </c>
+      <c r="E53" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" t="s">
+        <v>179</v>
+      </c>
+      <c r="D54" t="s">
+        <v>152</v>
+      </c>
+      <c r="E54" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" t="s">
+        <v>179</v>
+      </c>
+      <c r="D55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E55" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" t="s">
+        <v>179</v>
+      </c>
+      <c r="D57" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" t="s">
+        <v>179</v>
+      </c>
+      <c r="D58" t="s">
+        <v>152</v>
+      </c>
+      <c r="E58" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" t="s">
+        <v>179</v>
+      </c>
+      <c r="D59" t="s">
+        <v>152</v>
+      </c>
+      <c r="F59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4341AC-9278-4308-B637-81E7010F9C46}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -2005,7 +3947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F5497E-3E08-4F53-A7A4-FF5A523F6922}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2097,7 +4039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82253B5-151F-4D3E-BE53-1427E1059EE2}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2211,11 +4153,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECFEABF-1827-41A5-9CBF-DD0F4CBE752D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2328,11 +4270,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1026899-EDF0-43C7-8585-EB7C14354B18}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -2820,4 +4762,174 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9673C06D-0E7A-4BB1-9BEC-1A1D6219C856}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5005DDF-E2BC-4A3E-B667-90F5CBFB6BB1}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed and tested chapter 1 pipeline
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_1.xlsx
+++ b/data/templates/dukes_ch_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7604F51-DB38-41F2-891A-6ECAEEA42398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFE7F6B5-465C-4523-B95E-42A5BB7EA719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="10" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="1.2" sheetId="11" r:id="rId3"/>
     <sheet name="1.3.A" sheetId="1" r:id="rId4"/>
     <sheet name="1.3.B" sheetId="3" r:id="rId5"/>
-    <sheet name="1.1.A" sheetId="4" r:id="rId6"/>
-    <sheet name="1.1.B" sheetId="5" r:id="rId7"/>
-    <sheet name="1.1.C" sheetId="6" r:id="rId8"/>
+    <sheet name="1.1.1.A" sheetId="4" r:id="rId6"/>
+    <sheet name="1.1.1.B" sheetId="5" r:id="rId7"/>
+    <sheet name="1.1.1.C" sheetId="6" r:id="rId8"/>
     <sheet name="1.1.2" sheetId="2" r:id="rId9"/>
     <sheet name="1.1.3" sheetId="7" r:id="rId10"/>
     <sheet name="1.1.4" sheetId="8" r:id="rId11"/>
@@ -3481,7 +3481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC8CCF9-B8CA-4BD3-B98A-FD35E301146D}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
@@ -6821,8 +6821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECFEABF-1827-41A5-9CBF-DD0F4CBE752D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Transformer functions now set the index
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_1.xlsx
+++ b/data/templates/dukes_ch_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684DEBCD-6829-44F1-9FBB-3F7DBE41CC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122299F0-3CBC-4F05-BB2F-46016DE0C0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="11" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="212">
   <si>
     <t>Electricity generation - Gas</t>
   </si>
@@ -549,9 +549,6 @@
   </si>
   <si>
     <t>Supply</t>
-  </si>
-  <si>
-    <t>type</t>
   </si>
   <si>
     <t>Statistical difference</t>
@@ -1673,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D05EE7-8D8D-45F8-9599-5A89EAB3B8C2}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1704,7 +1701,7 @@
         <v>78</v>
       </c>
       <c r="G1" t="s">
-        <v>171</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1726,6 +1723,9 @@
       <c r="F2" t="s">
         <v>40</v>
       </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1746,6 +1746,9 @@
       <c r="F3" t="s">
         <v>41</v>
       </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -1766,6 +1769,9 @@
       <c r="F4" t="s">
         <v>42</v>
       </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1786,6 +1792,9 @@
       <c r="F5" t="s">
         <v>43</v>
       </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -1798,13 +1807,16 @@
         <v>170</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
-        <v>174</v>
+        <v>173</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1826,6 +1838,9 @@
       <c r="F7" t="s">
         <v>170</v>
       </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1835,16 +1850,19 @@
         <v>129</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F8" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1855,16 +1873,19 @@
         <v>130</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>172</v>
+      </c>
+      <c r="G9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1875,7 +1896,7 @@
         <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D10" t="s">
         <v>131</v>
@@ -1885,6 +1906,9 @@
       </c>
       <c r="F10" t="s">
         <v>131</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1895,7 +1919,7 @@
         <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
         <v>132</v>
@@ -1905,6 +1929,9 @@
       </c>
       <c r="F11" t="s">
         <v>132</v>
+      </c>
+      <c r="G11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1915,7 +1942,7 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
         <v>132</v>
@@ -1925,6 +1952,9 @@
       </c>
       <c r="F12" t="s">
         <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1935,7 +1965,7 @@
         <v>133</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D13" t="s">
         <v>132</v>
@@ -1945,6 +1975,9 @@
       </c>
       <c r="F13" t="s">
         <v>133</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1955,7 +1988,7 @@
         <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D14" t="s">
         <v>132</v>
@@ -1965,6 +1998,9 @@
       </c>
       <c r="F14" t="s">
         <v>134</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1975,7 +2011,7 @@
         <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D15" t="s">
         <v>132</v>
@@ -1985,6 +2021,9 @@
       </c>
       <c r="F15" t="s">
         <v>135</v>
+      </c>
+      <c r="G15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1995,7 +2034,7 @@
         <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D16" t="s">
         <v>132</v>
@@ -2006,8 +2045,11 @@
       <c r="F16" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2015,7 +2057,7 @@
         <v>137</v>
       </c>
       <c r="C17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D17" t="s">
         <v>132</v>
@@ -2026,8 +2068,11 @@
       <c r="F17" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2035,7 +2080,7 @@
         <v>138</v>
       </c>
       <c r="C18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D18" t="s">
         <v>132</v>
@@ -2046,8 +2091,11 @@
       <c r="F18" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2055,7 +2103,7 @@
         <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
@@ -2066,8 +2114,11 @@
       <c r="F19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2075,7 +2126,7 @@
         <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D20" t="s">
         <v>132</v>
@@ -2086,8 +2137,11 @@
       <c r="F20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2095,7 +2149,7 @@
         <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
         <v>141</v>
@@ -2106,8 +2160,11 @@
       <c r="F21" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2115,7 +2172,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D22" t="s">
         <v>141</v>
@@ -2126,8 +2183,11 @@
       <c r="F22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2135,7 +2195,7 @@
         <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D23" t="s">
         <v>141</v>
@@ -2146,8 +2206,11 @@
       <c r="F23" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2155,7 +2218,7 @@
         <v>136</v>
       </c>
       <c r="C24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D24" t="s">
         <v>141</v>
@@ -2166,8 +2229,11 @@
       <c r="F24" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2175,7 +2241,7 @@
         <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D25" t="s">
         <v>141</v>
@@ -2186,8 +2252,11 @@
       <c r="F25" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2195,7 +2264,7 @@
         <v>137</v>
       </c>
       <c r="C26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D26" t="s">
         <v>141</v>
@@ -2206,8 +2275,11 @@
       <c r="F26" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2215,7 +2287,7 @@
         <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D27" t="s">
         <v>141</v>
@@ -2226,8 +2298,11 @@
       <c r="F27" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2235,7 +2310,7 @@
         <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D28" t="s">
         <v>141</v>
@@ -2246,8 +2321,11 @@
       <c r="F28" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2255,19 +2333,22 @@
         <v>144</v>
       </c>
       <c r="C29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D29" t="s">
         <v>141</v>
       </c>
       <c r="E29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F29" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+      <c r="G29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2275,7 +2356,7 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D30" t="s">
         <v>141</v>
@@ -2286,8 +2367,11 @@
       <c r="F30" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2295,7 +2379,7 @@
         <v>145</v>
       </c>
       <c r="C31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D31" t="s">
         <v>145</v>
@@ -2306,8 +2390,11 @@
       <c r="F31" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2315,7 +2402,7 @@
         <v>146</v>
       </c>
       <c r="C32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D32" t="s">
         <v>146</v>
@@ -2326,8 +2413,11 @@
       <c r="F32" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2335,7 +2425,7 @@
         <v>118</v>
       </c>
       <c r="C33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D33" t="s">
         <v>146</v>
@@ -2346,8 +2436,11 @@
       <c r="F33" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2355,7 +2448,7 @@
         <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D34" t="s">
         <v>146</v>
@@ -2366,8 +2459,11 @@
       <c r="F34" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2375,7 +2471,7 @@
         <v>148</v>
       </c>
       <c r="C35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D35" t="s">
         <v>146</v>
@@ -2386,8 +2482,11 @@
       <c r="F35" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2395,7 +2494,7 @@
         <v>149</v>
       </c>
       <c r="C36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D36" t="s">
         <v>146</v>
@@ -2406,8 +2505,11 @@
       <c r="F36" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2415,7 +2517,7 @@
         <v>150</v>
       </c>
       <c r="C37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D37" t="s">
         <v>146</v>
@@ -2426,8 +2528,11 @@
       <c r="F37" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2435,7 +2540,7 @@
         <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D38" t="s">
         <v>146</v>
@@ -2446,8 +2551,11 @@
       <c r="F38" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2455,7 +2563,7 @@
         <v>152</v>
       </c>
       <c r="C39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D39" t="s">
         <v>146</v>
@@ -2466,8 +2574,11 @@
       <c r="F39" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2475,7 +2586,7 @@
         <v>153</v>
       </c>
       <c r="C40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D40" t="s">
         <v>146</v>
@@ -2486,8 +2597,11 @@
       <c r="F40" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2495,7 +2609,7 @@
         <v>154</v>
       </c>
       <c r="C41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D41" t="s">
         <v>146</v>
@@ -2506,8 +2620,11 @@
       <c r="F41" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2515,7 +2632,7 @@
         <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D42" t="s">
         <v>146</v>
@@ -2526,8 +2643,11 @@
       <c r="F42" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2535,7 +2655,7 @@
         <v>156</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D43" t="s">
         <v>146</v>
@@ -2546,8 +2666,11 @@
       <c r="F43" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2555,7 +2678,7 @@
         <v>157</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D44" t="s">
         <v>146</v>
@@ -2566,8 +2689,11 @@
       <c r="F44" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2575,7 +2701,7 @@
         <v>158</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D45" t="s">
         <v>146</v>
@@ -2586,8 +2712,11 @@
       <c r="F45" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2595,7 +2724,7 @@
         <v>159</v>
       </c>
       <c r="C46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D46" t="s">
         <v>146</v>
@@ -2606,8 +2735,11 @@
       <c r="F46" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2615,7 +2747,7 @@
         <v>28</v>
       </c>
       <c r="C47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D47" t="s">
         <v>146</v>
@@ -2626,8 +2758,11 @@
       <c r="F47" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2635,7 +2770,7 @@
         <v>160</v>
       </c>
       <c r="C48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D48" t="s">
         <v>146</v>
@@ -2646,8 +2781,11 @@
       <c r="F48" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2655,7 +2793,7 @@
         <v>161</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D49" t="s">
         <v>146</v>
@@ -2666,8 +2804,11 @@
       <c r="F49" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2675,7 +2816,7 @@
         <v>162</v>
       </c>
       <c r="C50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D50" t="s">
         <v>146</v>
@@ -2686,8 +2827,11 @@
       <c r="F50" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2695,7 +2839,7 @@
         <v>163</v>
       </c>
       <c r="C51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
         <v>146</v>
@@ -2706,8 +2850,11 @@
       <c r="F51" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2715,7 +2862,7 @@
         <v>164</v>
       </c>
       <c r="C52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D52" t="s">
         <v>146</v>
@@ -2726,8 +2873,11 @@
       <c r="F52" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2735,7 +2885,7 @@
         <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D53" t="s">
         <v>146</v>
@@ -2746,8 +2896,11 @@
       <c r="F53" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2755,7 +2908,7 @@
         <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D54" t="s">
         <v>146</v>
@@ -2766,8 +2919,11 @@
       <c r="F54" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2775,7 +2931,7 @@
         <v>165</v>
       </c>
       <c r="C55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D55" t="s">
         <v>146</v>
@@ -2786,8 +2942,11 @@
       <c r="F55" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2795,7 +2954,7 @@
         <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D56" t="s">
         <v>146</v>
@@ -2806,8 +2965,11 @@
       <c r="F56" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2815,7 +2977,7 @@
         <v>26</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D57" t="s">
         <v>146</v>
@@ -2826,8 +2988,11 @@
       <c r="F57" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2835,7 +3000,7 @@
         <v>166</v>
       </c>
       <c r="C58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D58" t="s">
         <v>146</v>
@@ -2846,8 +3011,11 @@
       <c r="F58" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2855,7 +3023,7 @@
         <v>47</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D59" t="s">
         <v>146</v>
@@ -2865,6 +3033,9 @@
       </c>
       <c r="F59" t="s">
         <v>47</v>
+      </c>
+      <c r="G59" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3046,8 +3217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D425282C-868D-490E-98D9-DD5403F8543C}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3576,10 +3747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC8CCF9-B8CA-4BD3-B98A-FD35E301146D}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3588,7 +3759,7 @@
     <col min="3" max="3" width="42.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3610,13 +3781,16 @@
       <c r="G1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
@@ -3634,7 +3808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3657,7 +3831,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3680,7 +3854,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3703,12 +3877,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
         <v>127</v>
@@ -3717,21 +3891,21 @@
         <v>170</v>
       </c>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C7" t="s">
         <v>128</v>
@@ -3749,53 +3923,53 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8" t="s">
         <v>129</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C9" t="s">
         <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3806,7 +3980,7 @@
         <v>131</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E10" t="s">
         <v>131</v>
@@ -3818,7 +3992,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3829,7 +4003,7 @@
         <v>132</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E11" t="s">
         <v>132</v>
@@ -3841,7 +4015,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3852,7 +4026,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E12" t="s">
         <v>132</v>
@@ -3864,7 +4038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3875,7 +4049,7 @@
         <v>133</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" t="s">
         <v>132</v>
@@ -3887,7 +4061,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3898,7 +4072,7 @@
         <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E14" t="s">
         <v>132</v>
@@ -3910,7 +4084,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3921,7 +4095,7 @@
         <v>135</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E15" t="s">
         <v>132</v>
@@ -3930,21 +4104,21 @@
         <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E16" t="s">
         <v>132</v>
@@ -3953,7 +4127,7 @@
         <v>135</v>
       </c>
       <c r="G16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3967,7 +4141,7 @@
         <v>136</v>
       </c>
       <c r="D17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E17" t="s">
         <v>132</v>
@@ -3990,7 +4164,7 @@
         <v>137</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E18" t="s">
         <v>132</v>
@@ -4013,7 +4187,7 @@
         <v>138</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E19" t="s">
         <v>132</v>
@@ -4036,7 +4210,7 @@
         <v>139</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E20" t="s">
         <v>132</v>
@@ -4059,7 +4233,7 @@
         <v>140</v>
       </c>
       <c r="D21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E21" t="s">
         <v>132</v>
@@ -4082,7 +4256,7 @@
         <v>141</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E22" t="s">
         <v>141</v>
@@ -4105,7 +4279,7 @@
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E23" t="s">
         <v>141</v>
@@ -4128,7 +4302,7 @@
         <v>142</v>
       </c>
       <c r="D24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E24" t="s">
         <v>141</v>
@@ -4151,7 +4325,7 @@
         <v>136</v>
       </c>
       <c r="D25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
         <v>141</v>
@@ -4174,7 +4348,7 @@
         <v>143</v>
       </c>
       <c r="D26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E26" t="s">
         <v>141</v>
@@ -4197,7 +4371,7 @@
         <v>137</v>
       </c>
       <c r="D27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E27" t="s">
         <v>141</v>
@@ -4220,7 +4394,7 @@
         <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E28" t="s">
         <v>141</v>
@@ -4243,7 +4417,7 @@
         <v>139</v>
       </c>
       <c r="D29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E29" t="s">
         <v>141</v>
@@ -4260,22 +4434,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C30" t="s">
         <v>144</v>
       </c>
       <c r="D30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E30" t="s">
         <v>141</v>
       </c>
       <c r="F30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4289,7 +4463,7 @@
         <v>21</v>
       </c>
       <c r="D31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E31" t="s">
         <v>141</v>
@@ -4312,7 +4486,7 @@
         <v>145</v>
       </c>
       <c r="D32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E32" t="s">
         <v>145</v>
@@ -4335,7 +4509,7 @@
         <v>146</v>
       </c>
       <c r="D33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E33" t="s">
         <v>146</v>
@@ -4358,7 +4532,7 @@
         <v>118</v>
       </c>
       <c r="D34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E34" t="s">
         <v>146</v>
@@ -4381,7 +4555,7 @@
         <v>147</v>
       </c>
       <c r="D35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E35" t="s">
         <v>146</v>
@@ -4404,7 +4578,7 @@
         <v>148</v>
       </c>
       <c r="D36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E36" t="s">
         <v>146</v>
@@ -4427,7 +4601,7 @@
         <v>149</v>
       </c>
       <c r="D37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E37" t="s">
         <v>146</v>
@@ -4450,7 +4624,7 @@
         <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E38" t="s">
         <v>146</v>
@@ -4473,7 +4647,7 @@
         <v>151</v>
       </c>
       <c r="D39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E39" t="s">
         <v>146</v>
@@ -4496,7 +4670,7 @@
         <v>152</v>
       </c>
       <c r="D40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E40" t="s">
         <v>146</v>
@@ -4519,7 +4693,7 @@
         <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E41" t="s">
         <v>146</v>
@@ -4542,7 +4716,7 @@
         <v>154</v>
       </c>
       <c r="D42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E42" t="s">
         <v>146</v>
@@ -4565,7 +4739,7 @@
         <v>155</v>
       </c>
       <c r="D43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E43" t="s">
         <v>146</v>
@@ -4588,7 +4762,7 @@
         <v>156</v>
       </c>
       <c r="D44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E44" t="s">
         <v>146</v>
@@ -4611,7 +4785,7 @@
         <v>157</v>
       </c>
       <c r="D45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E45" t="s">
         <v>146</v>
@@ -4634,7 +4808,7 @@
         <v>158</v>
       </c>
       <c r="D46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E46" t="s">
         <v>146</v>
@@ -4657,7 +4831,7 @@
         <v>159</v>
       </c>
       <c r="D47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E47" t="s">
         <v>146</v>
@@ -4674,13 +4848,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C48" t="s">
         <v>28</v>
       </c>
       <c r="D48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E48" t="s">
         <v>146</v>
@@ -4703,7 +4877,7 @@
         <v>160</v>
       </c>
       <c r="D49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E49" t="s">
         <v>146</v>
@@ -4726,7 +4900,7 @@
         <v>161</v>
       </c>
       <c r="D50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E50" t="s">
         <v>146</v>
@@ -4749,7 +4923,7 @@
         <v>162</v>
       </c>
       <c r="D51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E51" t="s">
         <v>146</v>
@@ -4772,7 +4946,7 @@
         <v>163</v>
       </c>
       <c r="D52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E52" t="s">
         <v>146</v>
@@ -4795,7 +4969,7 @@
         <v>164</v>
       </c>
       <c r="D53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E53" t="s">
         <v>146</v>
@@ -4818,7 +4992,7 @@
         <v>21</v>
       </c>
       <c r="D54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E54" t="s">
         <v>146</v>
@@ -4841,7 +5015,7 @@
         <v>30</v>
       </c>
       <c r="D55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E55" t="s">
         <v>146</v>
@@ -4864,7 +5038,7 @@
         <v>165</v>
       </c>
       <c r="D56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E56" t="s">
         <v>146</v>
@@ -4887,7 +5061,7 @@
         <v>27</v>
       </c>
       <c r="D57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E57" t="s">
         <v>146</v>
@@ -4910,7 +5084,7 @@
         <v>26</v>
       </c>
       <c r="D58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E58" t="s">
         <v>146</v>
@@ -4933,7 +5107,7 @@
         <v>166</v>
       </c>
       <c r="D59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E59" t="s">
         <v>146</v>
@@ -4956,7 +5130,7 @@
         <v>47</v>
       </c>
       <c r="D60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E60" t="s">
         <v>146</v>
@@ -4970,7 +5144,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E61" t="s">
         <v>146</v>
@@ -4988,8 +5162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DF71E3-D330-4248-A0E3-2256A1167A8F}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5046,16 +5220,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
@@ -5067,16 +5241,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
@@ -5109,16 +5283,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -5130,16 +5304,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
@@ -5151,16 +5325,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
@@ -5175,7 +5349,7 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
@@ -5193,13 +5367,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E10" t="s">
         <v>125</v>
@@ -5214,16 +5388,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" t="s">
         <v>200</v>
-      </c>
-      <c r="D11" t="s">
-        <v>180</v>
-      </c>
-      <c r="E11" t="s">
-        <v>201</v>
       </c>
       <c r="F11" t="s">
         <v>34</v>
@@ -5235,16 +5409,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
@@ -5256,16 +5430,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
@@ -5277,16 +5451,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F14" t="s">
         <v>34</v>
@@ -5298,16 +5472,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F15" t="s">
         <v>34</v>
@@ -5322,7 +5496,7 @@
         <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
         <v>124</v>
@@ -5343,7 +5517,7 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D17" t="s">
         <v>30</v>
@@ -5364,7 +5538,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
@@ -5382,16 +5556,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F19" t="s">
         <v>34</v>
@@ -5406,7 +5580,7 @@
         <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D20" t="s">
         <v>47</v>
@@ -5424,16 +5598,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F21" t="s">
         <v>34</v>
@@ -5448,7 +5622,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
@@ -5466,16 +5640,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F23" t="s">
         <v>34</v>
@@ -5487,16 +5661,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
@@ -5508,16 +5682,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F25" t="s">
         <v>34</v>
@@ -5529,16 +5703,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F26" t="s">
         <v>34</v>
@@ -5553,7 +5727,7 @@
         <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D27" t="s">
         <v>124</v>
@@ -5574,7 +5748,7 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -5595,7 +5769,7 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D29" t="s">
         <v>26</v>
@@ -5613,16 +5787,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C30" t="s">
         <v>186</v>
       </c>
-      <c r="C30" t="s">
-        <v>187</v>
-      </c>
       <c r="D30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
@@ -5634,16 +5808,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F31" t="s">
         <v>34</v>
@@ -5655,16 +5829,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F32" t="s">
         <v>34</v>
@@ -5676,16 +5850,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F33" t="s">
         <v>34</v>
@@ -5697,16 +5871,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" t="s">
         <v>190</v>
       </c>
-      <c r="D34" t="s">
-        <v>191</v>
-      </c>
       <c r="E34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F34" t="s">
         <v>34</v>
@@ -5721,7 +5895,7 @@
         <v>132</v>
       </c>
       <c r="C35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D35" t="s">
         <v>132</v>
@@ -5742,7 +5916,7 @@
         <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D36" t="s">
         <v>19</v>
@@ -5760,16 +5934,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C37" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D37" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E37" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F37" t="s">
         <v>34</v>
@@ -5784,7 +5958,7 @@
         <v>135</v>
       </c>
       <c r="C38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D38" t="s">
         <v>135</v>
@@ -5805,7 +5979,7 @@
         <v>136</v>
       </c>
       <c r="C39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D39" t="s">
         <v>136</v>
@@ -5823,13 +5997,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E40" t="s">
         <v>125</v>
@@ -5844,16 +6018,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F41" t="s">
         <v>34</v>
@@ -5865,16 +6039,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F42" t="s">
         <v>34</v>
@@ -5886,16 +6060,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C43" t="s">
+        <v>192</v>
+      </c>
+      <c r="D43" t="s">
         <v>193</v>
       </c>
-      <c r="D43" t="s">
-        <v>194</v>
-      </c>
       <c r="E43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F43" t="s">
         <v>34</v>
@@ -5910,7 +6084,7 @@
         <v>136</v>
       </c>
       <c r="C44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D44" t="s">
         <v>136</v>
@@ -5931,7 +6105,7 @@
         <v>143</v>
       </c>
       <c r="C45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D45" t="s">
         <v>143</v>
@@ -5949,16 +6123,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F46" t="s">
         <v>34</v>
@@ -5970,16 +6144,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F47" t="s">
         <v>34</v>
@@ -5997,10 +6171,10 @@
         <v>118</v>
       </c>
       <c r="D48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F48" t="s">
         <v>34</v>
@@ -6012,16 +6186,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C49" t="s">
         <v>118</v>
       </c>
       <c r="D49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F49" t="s">
         <v>34</v>
@@ -6033,16 +6207,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C50" t="s">
         <v>118</v>
       </c>
       <c r="D50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F50" t="s">
         <v>34</v>
@@ -6060,10 +6234,10 @@
         <v>28</v>
       </c>
       <c r="D51" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E51" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F51" t="s">
         <v>34</v>
@@ -6075,16 +6249,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C52" t="s">
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E52" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F52" t="s">
         <v>34</v>
@@ -6096,16 +6270,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C53" t="s">
         <v>28</v>
       </c>
       <c r="D53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F53" t="s">
         <v>34</v>
@@ -6144,10 +6318,10 @@
         <v>123</v>
       </c>
       <c r="D55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F55" t="s">
         <v>34</v>
@@ -6201,16 +6375,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C58" t="s">
         <v>123</v>
       </c>
       <c r="D58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F58" t="s">
         <v>34</v>
@@ -6222,16 +6396,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F59" t="s">
         <v>34</v>
@@ -6243,16 +6417,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F60" t="s">
         <v>34</v>
@@ -6264,16 +6438,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F61" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Further improvements for DUKES 1.1.5 and other debugging
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_1.xlsx
+++ b/data/templates/dukes_ch_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122299F0-3CBC-4F05-BB2F-46016DE0C0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A382768-7532-498E-868A-06B22D025323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="11" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="218">
   <si>
     <t>Electricity generation - Gas</t>
   </si>
@@ -672,6 +672,24 @@
   </si>
   <si>
     <t>All plants</t>
+  </si>
+  <si>
+    <t>Coal [note 1]</t>
+  </si>
+  <si>
+    <t>Petroleum [note 2]</t>
+  </si>
+  <si>
+    <t>Natural gas [note 3]</t>
+  </si>
+  <si>
+    <t>Nuclear electricity [note 4]</t>
+  </si>
+  <si>
+    <t>Wind, solar and hydro electricity [note 4] [note 5]</t>
+  </si>
+  <si>
+    <t>Total [note 6]</t>
   </si>
 </sst>
 </file>
@@ -3217,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D425282C-868D-490E-98D9-DD5403F8543C}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5162,7 +5180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DF71E3-D330-4248-A0E3-2256A1167A8F}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -7213,81 +7231,99 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F5497E-3E08-4F53-A7A4-FF5A523F6922}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D8" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>117</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7295,7 +7331,20 @@
         <v>63</v>
       </c>
       <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -7305,81 +7354,99 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82253B5-151F-4D3E-BE53-1427E1059EE2}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>117</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7387,10 +7454,13 @@
         <v>63</v>
       </c>
       <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -7398,17 +7468,23 @@
         <v>68</v>
       </c>
       <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7419,84 +7495,102 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECFEABF-1827-41A5-9CBF-DD0F4CBE752D}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>117</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7504,10 +7598,13 @@
         <v>63</v>
       </c>
       <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -7515,17 +7612,23 @@
         <v>68</v>
       </c>
       <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed duplicate label columns from J.1 template
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_1.xlsx
+++ b/data/templates/dukes_ch_1.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A382768-7532-498E-868A-06B22D025323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7719344-84DB-4FFF-AD98-0E41C314B7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="11" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="10" r:id="rId1"/>
-    <sheet name="J.1" sheetId="12" r:id="rId2"/>
-    <sheet name="1.2" sheetId="11" r:id="rId3"/>
-    <sheet name="1.3.A" sheetId="1" r:id="rId4"/>
-    <sheet name="1.3.B" sheetId="3" r:id="rId5"/>
-    <sheet name="1.1.1.A" sheetId="4" r:id="rId6"/>
-    <sheet name="1.1.1.B" sheetId="5" r:id="rId7"/>
-    <sheet name="1.1.1.C" sheetId="6" r:id="rId8"/>
-    <sheet name="1.1.2" sheetId="2" r:id="rId9"/>
-    <sheet name="1.1.3" sheetId="7" r:id="rId10"/>
-    <sheet name="1.1.4" sheetId="8" r:id="rId11"/>
-    <sheet name="1.1.6" sheetId="9" r:id="rId12"/>
+    <sheet name="I.1" sheetId="13" r:id="rId2"/>
+    <sheet name="J.1" sheetId="12" r:id="rId3"/>
+    <sheet name="1.2" sheetId="11" r:id="rId4"/>
+    <sheet name="1.3.A" sheetId="1" r:id="rId5"/>
+    <sheet name="1.3.B" sheetId="3" r:id="rId6"/>
+    <sheet name="1.1.1.A" sheetId="4" r:id="rId7"/>
+    <sheet name="1.1.1.B" sheetId="5" r:id="rId8"/>
+    <sheet name="1.1.1.C" sheetId="6" r:id="rId9"/>
+    <sheet name="1.1.2" sheetId="2" r:id="rId10"/>
+    <sheet name="1.1.3" sheetId="7" r:id="rId11"/>
+    <sheet name="1.1.4" sheetId="8" r:id="rId12"/>
+    <sheet name="1.1.6" sheetId="9" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="218">
   <si>
     <t>Electricity generation - Gas</t>
   </si>
@@ -3062,6 +3063,500 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1026899-EDF0-43C7-8585-EB7C14354B18}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9673C06D-0E7A-4BB1-9BEC-1A1D6219C856}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3146,7 +3641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5005DDF-E2BC-4A3E-B667-90F5CBFB6BB1}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3231,12 +3726,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D425282C-868D-490E-98D9-DD5403F8543C}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A27" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3764,20 +4259,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC8CCF9-B8CA-4BD3-B98A-FD35E301146D}">
-  <dimension ref="A1:H61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732E0C56-183C-4199-8E1E-44BA09BFCEE6}">
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="C19" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.88671875" customWidth="1"/>
-    <col min="3" max="3" width="42.88671875" customWidth="1"/>
+    <col min="2" max="2" width="53.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3785,36 +4281,33 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F1" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>170</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>
@@ -3823,10 +4316,10 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3834,10 +4327,10 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>170</v>
       </c>
       <c r="E3" t="s">
         <v>41</v>
@@ -3846,10 +4339,10 @@
         <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3857,10 +4350,10 @@
         <v>42</v>
       </c>
       <c r="C4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" t="s">
         <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>170</v>
       </c>
       <c r="E4" t="s">
         <v>42</v>
@@ -3869,10 +4362,10 @@
         <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3880,10 +4373,10 @@
         <v>43</v>
       </c>
       <c r="C5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>170</v>
       </c>
       <c r="E5" t="s">
         <v>43</v>
@@ -3892,21 +4385,21 @@
         <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" t="s">
         <v>173</v>
-      </c>
-      <c r="C6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" t="s">
-        <v>170</v>
       </c>
       <c r="E6" t="s">
         <v>173</v>
@@ -3915,18 +4408,18 @@
         <v>173</v>
       </c>
       <c r="G6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
         <v>170</v>
@@ -3938,18 +4431,18 @@
         <v>170</v>
       </c>
       <c r="G7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
         <v>171</v>
-      </c>
-      <c r="C8" t="s">
-        <v>129</v>
       </c>
       <c r="D8" t="s">
         <v>171</v>
@@ -3961,18 +4454,18 @@
         <v>171</v>
       </c>
       <c r="G8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
         <v>172</v>
@@ -3984,10 +4477,10 @@
         <v>172</v>
       </c>
       <c r="G9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3995,10 +4488,10 @@
         <v>131</v>
       </c>
       <c r="C10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" t="s">
         <v>131</v>
-      </c>
-      <c r="D10" t="s">
-        <v>172</v>
       </c>
       <c r="E10" t="s">
         <v>131</v>
@@ -4007,10 +4500,10 @@
         <v>131</v>
       </c>
       <c r="G10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4018,10 +4511,10 @@
         <v>132</v>
       </c>
       <c r="C11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" t="s">
         <v>132</v>
-      </c>
-      <c r="D11" t="s">
-        <v>172</v>
       </c>
       <c r="E11" t="s">
         <v>132</v>
@@ -4030,10 +4523,10 @@
         <v>132</v>
       </c>
       <c r="G11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4041,22 +4534,22 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>172</v>
-      </c>
-      <c r="E12" t="s">
-        <v>132</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4064,22 +4557,22 @@
         <v>133</v>
       </c>
       <c r="C13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
         <v>133</v>
       </c>
-      <c r="D13" t="s">
-        <v>172</v>
-      </c>
-      <c r="E13" t="s">
-        <v>132</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
       <c r="G13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4087,22 +4580,22 @@
         <v>134</v>
       </c>
       <c r="C14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
         <v>134</v>
       </c>
-      <c r="D14" t="s">
-        <v>172</v>
-      </c>
-      <c r="E14" t="s">
-        <v>132</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
       <c r="G14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4110,42 +4603,42 @@
         <v>135</v>
       </c>
       <c r="C15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" t="s">
         <v>135</v>
-      </c>
-      <c r="D15" t="s">
-        <v>172</v>
-      </c>
-      <c r="E15" t="s">
-        <v>132</v>
       </c>
       <c r="F15" t="s">
         <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
+        <v>172</v>
       </c>
       <c r="D16" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G16" t="s">
-        <v>210</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -4153,22 +4646,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G17" t="s">
-        <v>136</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -4176,22 +4669,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="D18" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="F18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G18" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -4199,22 +4692,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="D19" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G19" t="s">
-        <v>138</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -4222,22 +4715,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>139</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -4245,22 +4738,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>141</v>
       </c>
       <c r="G21" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -4268,22 +4761,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" t="s">
         <v>141</v>
       </c>
-      <c r="C22" t="s">
-        <v>141</v>
-      </c>
-      <c r="D22" t="s">
-        <v>172</v>
-      </c>
       <c r="E22" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="G22" t="s">
-        <v>141</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -4291,22 +4784,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>172</v>
       </c>
       <c r="D23" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -4314,22 +4807,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="D24" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E24" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F24" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G24" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -4337,22 +4830,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="D25" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E25" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F25" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="G25" t="s">
-        <v>136</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -4360,22 +4853,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C26" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F26" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G26" t="s">
-        <v>143</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -4383,22 +4876,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="D27" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G27" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -4406,22 +4899,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="D28" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G28" t="s">
-        <v>138</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -4429,22 +4922,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C29" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="D29" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E29" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="F29" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="G29" t="s">
-        <v>139</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -4452,22 +4945,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="D30" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E30" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="G30" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4475,22 +4968,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>172</v>
       </c>
       <c r="D31" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="G31" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -4498,22 +4991,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="D32" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E32" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F32" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G32" t="s">
-        <v>145</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4521,22 +5014,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" t="s">
         <v>146</v>
       </c>
-      <c r="C33" t="s">
-        <v>146</v>
-      </c>
-      <c r="D33" t="s">
-        <v>172</v>
-      </c>
       <c r="E33" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F33" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="G33" t="s">
-        <v>146</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4544,22 +5037,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" t="s">
         <v>118</v>
       </c>
-      <c r="C34" t="s">
-        <v>118</v>
-      </c>
-      <c r="D34" t="s">
-        <v>172</v>
-      </c>
-      <c r="E34" t="s">
-        <v>146</v>
-      </c>
       <c r="F34" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4567,22 +5060,22 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E35" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F35" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="G35" t="s">
-        <v>147</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4590,22 +5083,22 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C36" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="D36" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="G36" t="s">
-        <v>148</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4613,22 +5106,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="D37" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F37" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="G37" t="s">
-        <v>149</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4636,22 +5129,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="D38" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E38" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F38" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="G38" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4659,22 +5152,22 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="D39" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E39" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F39" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="G39" t="s">
-        <v>151</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4682,22 +5175,22 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F40" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="G40" t="s">
-        <v>152</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4705,22 +5198,22 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="D41" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E41" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F41" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="G41" t="s">
-        <v>153</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4728,22 +5221,22 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="D42" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E42" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F42" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="G42" t="s">
-        <v>154</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4751,22 +5244,22 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C43" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="D43" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E43" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F43" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="G43" t="s">
-        <v>155</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4774,22 +5267,22 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C44" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="D44" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E44" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F44" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="G44" t="s">
-        <v>156</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -4797,22 +5290,22 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C45" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="D45" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E45" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F45" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="G45" t="s">
-        <v>157</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4820,22 +5313,22 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C46" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="D46" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E46" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F46" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="G46" t="s">
-        <v>158</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -4843,22 +5336,22 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>28</v>
       </c>
       <c r="C47" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E47" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="F47" t="s">
-        <v>118</v>
+        <v>28</v>
       </c>
       <c r="G47" t="s">
-        <v>159</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4866,22 +5359,22 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>209</v>
+        <v>160</v>
       </c>
       <c r="C48" t="s">
+        <v>172</v>
+      </c>
+      <c r="D48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" t="s">
         <v>28</v>
       </c>
-      <c r="D48" t="s">
-        <v>172</v>
-      </c>
-      <c r="E48" t="s">
-        <v>146</v>
-      </c>
       <c r="F48" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="G48" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -4889,22 +5382,22 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C49" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="D49" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="F49" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="G49" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -4912,22 +5405,22 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C50" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="D50" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E50" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="F50" t="s">
-        <v>28</v>
+        <v>162</v>
       </c>
       <c r="G50" t="s">
-        <v>161</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -4935,22 +5428,22 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C51" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E51" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="F51" t="s">
-        <v>28</v>
+        <v>163</v>
       </c>
       <c r="G51" t="s">
-        <v>162</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -4958,22 +5451,22 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C52" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D52" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E52" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="F52" t="s">
-        <v>28</v>
+        <v>164</v>
       </c>
       <c r="G52" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -4981,22 +5474,22 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>164</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D53" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E53" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="F53" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G53" t="s">
-        <v>164</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -5004,22 +5497,22 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" t="s">
+        <v>146</v>
+      </c>
+      <c r="E54" t="s">
         <v>21</v>
       </c>
-      <c r="C54" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" t="s">
-        <v>172</v>
-      </c>
-      <c r="E54" t="s">
-        <v>146</v>
-      </c>
       <c r="F54" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G54" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -5027,22 +5520,22 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="C55" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="D55" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E55" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="F55" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="G55" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -5050,22 +5543,22 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>165</v>
+        <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D56" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E56" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="F56" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G56" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -5073,22 +5566,22 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="D57" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E57" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="F57" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G57" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -5096,22 +5589,22 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>166</v>
       </c>
       <c r="C58" t="s">
-        <v>26</v>
+        <v>172</v>
       </c>
       <c r="D58" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E58" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="F58" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="G58" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -5119,56 +5612,22 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>166</v>
+        <v>47</v>
       </c>
       <c r="C59" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D59" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E59" t="s">
-        <v>146</v>
+        <v>47</v>
       </c>
       <c r="F59" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G59" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>47</v>
-      </c>
-      <c r="C60" t="s">
-        <v>47</v>
-      </c>
-      <c r="D60" t="s">
-        <v>172</v>
-      </c>
-      <c r="E60" t="s">
-        <v>146</v>
-      </c>
-      <c r="F60" t="s">
-        <v>47</v>
-      </c>
-      <c r="G60" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D61" t="s">
-        <v>172</v>
-      </c>
-      <c r="E61" t="s">
-        <v>146</v>
-      </c>
-      <c r="G61" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -5177,6 +5636,1242 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC8CCF9-B8CA-4BD3-B98A-FD35E301146D}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" t="s">
+        <v>141</v>
+      </c>
+      <c r="E24" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" t="s">
+        <v>141</v>
+      </c>
+      <c r="E25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" t="s">
+        <v>141</v>
+      </c>
+      <c r="E26" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" t="s">
+        <v>172</v>
+      </c>
+      <c r="D27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" t="s">
+        <v>141</v>
+      </c>
+      <c r="E29" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" t="s">
+        <v>118</v>
+      </c>
+      <c r="F36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" t="s">
+        <v>172</v>
+      </c>
+      <c r="D38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" t="s">
+        <v>118</v>
+      </c>
+      <c r="F39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" t="s">
+        <v>146</v>
+      </c>
+      <c r="E40" t="s">
+        <v>118</v>
+      </c>
+      <c r="F40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" t="s">
+        <v>118</v>
+      </c>
+      <c r="F41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D42" t="s">
+        <v>146</v>
+      </c>
+      <c r="E42" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" t="s">
+        <v>172</v>
+      </c>
+      <c r="D43" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>157</v>
+      </c>
+      <c r="C45" t="s">
+        <v>172</v>
+      </c>
+      <c r="D45" t="s">
+        <v>146</v>
+      </c>
+      <c r="E45" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" t="s">
+        <v>172</v>
+      </c>
+      <c r="D46" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" t="s">
+        <v>118</v>
+      </c>
+      <c r="F46" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>159</v>
+      </c>
+      <c r="C47" t="s">
+        <v>172</v>
+      </c>
+      <c r="D47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" t="s">
+        <v>118</v>
+      </c>
+      <c r="F47" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>209</v>
+      </c>
+      <c r="C48" t="s">
+        <v>172</v>
+      </c>
+      <c r="D48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" t="s">
+        <v>146</v>
+      </c>
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>161</v>
+      </c>
+      <c r="C50" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" t="s">
+        <v>28</v>
+      </c>
+      <c r="F50" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>163</v>
+      </c>
+      <c r="C52" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" t="s">
+        <v>146</v>
+      </c>
+      <c r="E52" t="s">
+        <v>28</v>
+      </c>
+      <c r="F52" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" t="s">
+        <v>146</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" t="s">
+        <v>146</v>
+      </c>
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" t="s">
+        <v>172</v>
+      </c>
+      <c r="D55" t="s">
+        <v>146</v>
+      </c>
+      <c r="E55" t="s">
+        <v>21</v>
+      </c>
+      <c r="F55" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" t="s">
+        <v>146</v>
+      </c>
+      <c r="E56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" t="s">
+        <v>172</v>
+      </c>
+      <c r="D57" t="s">
+        <v>146</v>
+      </c>
+      <c r="E57" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" t="s">
+        <v>146</v>
+      </c>
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>166</v>
+      </c>
+      <c r="C59" t="s">
+        <v>172</v>
+      </c>
+      <c r="D59" t="s">
+        <v>146</v>
+      </c>
+      <c r="E59" t="s">
+        <v>21</v>
+      </c>
+      <c r="F59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" t="s">
+        <v>172</v>
+      </c>
+      <c r="D60" t="s">
+        <v>146</v>
+      </c>
+      <c r="E60" t="s">
+        <v>47</v>
+      </c>
+      <c r="F60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" t="s">
+        <v>146</v>
+      </c>
+      <c r="F61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToWidth="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DF71E3-D330-4248-A0E3-2256A1167A8F}">
   <dimension ref="A1:F61"/>
   <sheetViews>
@@ -6476,7 +8171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A95590D-4CE9-4A52-8AD4-52B5D68440D7}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -6854,7 +8549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4341AC-9278-4308-B637-81E7010F9C46}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -7229,7 +8924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F5497E-3E08-4F53-A7A4-FF5A523F6922}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -7352,7 +9047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82253B5-151F-4D3E-BE53-1427E1059EE2}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -7493,7 +9188,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECFEABF-1827-41A5-9CBF-DD0F4CBE752D}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -7635,498 +9330,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1026899-EDF0-43C7-8585-EB7C14354B18}">
-  <dimension ref="A1:E28"/>
-  <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished templates for all dukes
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_1.xlsx
+++ b/data/templates/dukes_ch_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7719344-84DB-4FFF-AD98-0E41C314B7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6007FD23-1CA6-42F4-8738-B2FA04AC0003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="10" r:id="rId1"/>
@@ -1689,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D05EE7-8D8D-45F8-9599-5A89EAB3B8C2}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C54" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5642,7 +5642,7 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>